<commit_message>
revise metadata and lit review
</commit_message>
<xml_diff>
--- a/results/tables/lit_review_covid19.xlsx
+++ b/results/tables/lit_review_covid19.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josephh\Documents\GitHub\hegsrr\RPr-Chakraborty2020\results\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilyz/Documents/GitHub/HEGSRR/RPr-Chakraborty-2021/results/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A1FBAE-296F-BE49-8305-2C9B2A1A6DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="765" yWindow="495" windowWidth="28035" windowHeight="16020"/>
+    <workbookView xWindow="800" yWindow="880" windowWidth="35560" windowHeight="19600" xr2:uid="{F7D3AAE0-CE18-5A4C-9029-858F6DF03216}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Raw Data</t>
   </si>
@@ -109,9 +110,6 @@
   </si>
   <si>
     <t>Impact of COVID-19 on services for people with disabilities and chronic health conditions</t>
-  </si>
-  <si>
-    <t>Brief report: The impact of the COVID-19 pandemic on health behaviors in adolescents with Autism Spectrum Disorder</t>
   </si>
   <si>
     <t>A cross-sectional analysis of trust of information and COVID-19 preventative practices among people with disabilities</t>
@@ -153,7 +151,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -507,24 +505,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08DD914-802A-2649-AFF7-4118777A11DA}">
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="128" customWidth="1"/>
-    <col min="2" max="2" width="18.875" customWidth="1"/>
-    <col min="3" max="3" width="31.125" customWidth="1"/>
-    <col min="4" max="4" width="26.375" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="22.125" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -541,10 +539,10 @@
         <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -552,7 +550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -560,7 +558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -568,7 +566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -576,7 +574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -584,7 +582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -592,7 +590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -603,7 +601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -611,7 +609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -622,7 +620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -630,7 +628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -638,7 +636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -646,7 +644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -654,7 +652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -662,7 +660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -670,7 +668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -678,7 +676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -686,7 +684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -694,63 +692,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>25</v>
       </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>19</v>
-      </c>
       <c r="B23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>26</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>28</v>
       </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -758,23 +756,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>30</v>
       </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -782,61 +780,53 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>33</v>
       </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>34</v>
       </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>35</v>
       </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
       <c r="C33">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>36</v>
-      </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B35">
-        <f>SUM(B2:B34)</f>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <f>SUM(B2:B33)</f>
         <v>7</v>
       </c>
-      <c r="C35">
-        <f t="shared" ref="C35:F35" si="0">SUM(C2:C34)</f>
-        <v>8</v>
-      </c>
-      <c r="D35">
+      <c r="C34">
+        <f t="shared" ref="C34:F34" si="0">SUM(C2:C33)</f>
+        <v>10</v>
+      </c>
+      <c r="D34">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="E35">
+        <v>16</v>
+      </c>
+      <c r="E34">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F35">
+      <c r="F34">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>